<commit_message>
some modifications but not completed
</commit_message>
<xml_diff>
--- a/kenya_sut/Database/Shock.xlsx
+++ b/kenya_sut/Database/Shock.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amin\Documents\GitHub\My Kenya\kenya_sut\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB7B447-776E-4790-972C-AFE7C586F762}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF012B1-EFA6-4FA0-8FD1-1B8F3B3B20CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E3629C0E-F9DC-4B74-958E-3933B88A68DB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E3629C0E-F9DC-4B74-958E-3933B88A68DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Y" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>level_row</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Coal</t>
+  </si>
+  <si>
+    <t>Maize (home consumed)</t>
   </si>
 </sst>
 </file>
@@ -474,8 +477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90C9F64B-C7F5-4AB9-AA62-A1FBBAFACE87}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,26 +498,24 @@
       <c r="A2" s="3">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1">
+        <v>100000000000000</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
+      <c r="A3" s="3"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
+      <c r="A4" s="3"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
+      <c r="A5" s="3"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
+      <c r="A6" s="3"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
@@ -528,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55614CFE-594E-42E2-8671-A16F08CAB202}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,7 +634,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Revert "Merge branch 'master' of https://github.com/FEEM-Africa-REP/CIVICS_Kenya"
This reverts commit ece37b0881dfd5daa6db89476ad6b8e2a69482ec, reversing
changes made to b4db9394526a06f7e1188d80cd83970677d1329d.
</commit_message>
<xml_diff>
--- a/kenya_sut/Database/Shock.xlsx
+++ b/kenya_sut/Database/Shock.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amin\Documents\GitHub\My Kenya\kenya_sut\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF012B1-EFA6-4FA0-8FD1-1B8F3B3B20CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB7B447-776E-4790-972C-AFE7C586F762}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E3629C0E-F9DC-4B74-958E-3933B88A68DB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E3629C0E-F9DC-4B74-958E-3933B88A68DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Y" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
   <si>
     <t>level_row</t>
   </si>
@@ -84,9 +84,6 @@
   </si>
   <si>
     <t>Coal</t>
-  </si>
-  <si>
-    <t>Maize (home consumed)</t>
   </si>
 </sst>
 </file>
@@ -477,8 +474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90C9F64B-C7F5-4AB9-AA62-A1FBBAFACE87}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,24 +495,26 @@
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="1">
-        <v>100000000000000</v>
-      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
@@ -529,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55614CFE-594E-42E2-8671-A16F08CAB202}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,7 +633,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Revert "Revert "Merge branch 'master' of https://github.com/FEEM-Africa-REP/CIVICS_Kenya""
This reverts commit 6fb3c46a9e6811a79a47c5f4b3d0d6469040a04f.
</commit_message>
<xml_diff>
--- a/kenya_sut/Database/Shock.xlsx
+++ b/kenya_sut/Database/Shock.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amin\Documents\GitHub\My Kenya\kenya_sut\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB7B447-776E-4790-972C-AFE7C586F762}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF012B1-EFA6-4FA0-8FD1-1B8F3B3B20CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E3629C0E-F9DC-4B74-958E-3933B88A68DB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E3629C0E-F9DC-4B74-958E-3933B88A68DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Y" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>level_row</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Coal</t>
+  </si>
+  <si>
+    <t>Maize (home consumed)</t>
   </si>
 </sst>
 </file>
@@ -474,8 +477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90C9F64B-C7F5-4AB9-AA62-A1FBBAFACE87}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,26 +498,24 @@
       <c r="A2" s="3">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1">
+        <v>100000000000000</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
+      <c r="A3" s="3"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
+      <c r="A4" s="3"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
+      <c r="A5" s="3"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
+      <c r="A6" s="3"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
@@ -528,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55614CFE-594E-42E2-8671-A16F08CAB202}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,7 +634,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Revert "Revert "Revert "Merge branch 'master' of https://github.com/FEEM-Africa-REP/CIVICS_Kenya"""
This reverts commit 81ffa24ef8a238d4e27288d975c955442b9ffa9c.
</commit_message>
<xml_diff>
--- a/kenya_sut/Database/Shock.xlsx
+++ b/kenya_sut/Database/Shock.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amin\Documents\GitHub\My Kenya\kenya_sut\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF012B1-EFA6-4FA0-8FD1-1B8F3B3B20CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB7B447-776E-4790-972C-AFE7C586F762}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E3629C0E-F9DC-4B74-958E-3933B88A68DB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E3629C0E-F9DC-4B74-958E-3933B88A68DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Y" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
   <si>
     <t>level_row</t>
   </si>
@@ -84,9 +84,6 @@
   </si>
   <si>
     <t>Coal</t>
-  </si>
-  <si>
-    <t>Maize (home consumed)</t>
   </si>
 </sst>
 </file>
@@ -477,8 +474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90C9F64B-C7F5-4AB9-AA62-A1FBBAFACE87}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,24 +495,26 @@
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="1">
-        <v>100000000000000</v>
-      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
@@ -529,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55614CFE-594E-42E2-8671-A16F08CAB202}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,7 +633,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
working on the new function of SHOCK
</commit_message>
<xml_diff>
--- a/kenya_sut/Database/Shock.xlsx
+++ b/kenya_sut/Database/Shock.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amin\Documents\GitHub\My Kenya\kenya_sut\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF012B1-EFA6-4FA0-8FD1-1B8F3B3B20CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{719A917D-F561-4640-BE8A-1B9D5F97E152}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E3629C0E-F9DC-4B74-958E-3933B88A68DB}"/>
+    <workbookView xWindow="4680" yWindow="1380" windowWidth="10440" windowHeight="6840" activeTab="1" xr2:uid="{E3629C0E-F9DC-4B74-958E-3933B88A68DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Y" sheetId="1" r:id="rId1"/>
-    <sheet name="A" sheetId="4" r:id="rId2"/>
+    <sheet name="Z" sheetId="4" r:id="rId2"/>
     <sheet name="VA" sheetId="5" r:id="rId3"/>
     <sheet name="E" sheetId="6" r:id="rId4"/>
   </sheets>
@@ -477,7 +477,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90C9F64B-C7F5-4AB9-AA62-A1FBBAFACE87}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -529,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55614CFE-594E-42E2-8671-A16F08CAB202}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,30 +588,22 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
+      <c r="A3" s="3"/>
       <c r="B3" s="2"/>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
+      <c r="A4" s="3"/>
       <c r="B4" s="2"/>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
+      <c r="A5" s="3"/>
       <c r="B5" s="2"/>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
+      <c r="A6" s="3"/>
       <c r="B6" s="2"/>
       <c r="D6" s="2"/>
     </row>

</xml_diff>

<commit_message>
Shock Function is done
</commit_message>
<xml_diff>
--- a/kenya_sut/Database/Shock.xlsx
+++ b/kenya_sut/Database/Shock.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amin\Documents\GitHub\My Kenya\kenya_sut\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{719A917D-F561-4640-BE8A-1B9D5F97E152}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC9A3264-8147-44FB-A28C-1F263CF573D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="1380" windowWidth="10440" windowHeight="6840" activeTab="1" xr2:uid="{E3629C0E-F9DC-4B74-958E-3933B88A68DB}"/>
+    <workbookView xWindow="10470" yWindow="7260" windowWidth="10440" windowHeight="6840" xr2:uid="{E3629C0E-F9DC-4B74-958E-3933B88A68DB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Y" sheetId="1" r:id="rId1"/>
-    <sheet name="Z" sheetId="4" r:id="rId2"/>
-    <sheet name="VA" sheetId="5" r:id="rId3"/>
-    <sheet name="E" sheetId="6" r:id="rId4"/>
+    <sheet name="S" sheetId="7" r:id="rId1"/>
+    <sheet name="Y" sheetId="1" r:id="rId2"/>
+    <sheet name="Z" sheetId="4" r:id="rId3"/>
+    <sheet name="VA" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
   <si>
     <t>level_row</t>
   </si>
@@ -78,12 +78,6 @@
   </si>
   <si>
     <t>Grain milling (production)</t>
-  </si>
-  <si>
-    <t>Non metallic products (production)</t>
-  </si>
-  <si>
-    <t>Coal</t>
   </si>
   <si>
     <t>Maize (home consumed)</t>
@@ -136,7 +130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -154,9 +148,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -474,6 +465,76 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{841E6236-0FE3-4A5E-9CF9-604E8F9DE95C}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="29" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{8DA3BBAC-AFCE-4BA5-A79C-4FF1BC61FE1B}">
+      <formula1>"Percentage, Absolute"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90C9F64B-C7F5-4AB9-AA62-A1FBBAFACE87}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -499,7 +560,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1">
         <v>100000000000000</v>
@@ -525,12 +586,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55614CFE-594E-42E2-8671-A16F08CAB202}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,7 +629,7 @@
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="6" t="s">
@@ -621,12 +682,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A46AE03-F2C9-4017-8F33-B063B461D8FD}">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A3" sqref="A3:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,24 +738,16 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
+      <c r="A3" s="3"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
+      <c r="A4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
+      <c r="A5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
+      <c r="A6" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -707,85 +760,4 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{213CD491-6ACF-4DEF-AA44-9822C20B2AB9}">
-  <dimension ref="A1:E7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="9.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{21DC3A67-B448-4C91-9B26-8041F6779EBD}">
-      <formula1>"Percentage, Absolute"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Modifications on the plots and shock functions and errors
</commit_message>
<xml_diff>
--- a/kenya_sut/Database/Shock.xlsx
+++ b/kenya_sut/Database/Shock.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amin\Documents\GitHub\My Kenya\kenya_sut\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC9A3264-8147-44FB-A28C-1F263CF573D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0396D0FF-7776-413D-BBAA-241364A0041C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10470" yWindow="7260" windowWidth="10440" windowHeight="6840" xr2:uid="{E3629C0E-F9DC-4B74-958E-3933B88A68DB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E3629C0E-F9DC-4B74-958E-3933B88A68DB}"/>
   </bookViews>
   <sheets>
     <sheet name="S" sheetId="7" r:id="rId1"/>
@@ -468,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{841E6236-0FE3-4A5E-9CF9-604E8F9DE95C}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,12 +539,15 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -590,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55614CFE-594E-42E2-8671-A16F08CAB202}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,13 +633,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>6</v>
@@ -645,7 +648,7 @@
         <v>9</v>
       </c>
       <c r="G2" s="5">
-        <v>0.5</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Some modifications on Shock Excel
</commit_message>
<xml_diff>
--- a/kenya_sut/Database/Shock.xlsx
+++ b/kenya_sut/Database/Shock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amin\Documents\GitHub\My Kenya\kenya_sut\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0396D0FF-7776-413D-BBAA-241364A0041C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C142D8C-57E7-4A3D-BBF3-CE0C1D4BC3A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E3629C0E-F9DC-4B74-958E-3933B88A68DB}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="Y" sheetId="1" r:id="rId2"/>
     <sheet name="Z" sheetId="4" r:id="rId3"/>
     <sheet name="VA" sheetId="5" r:id="rId4"/>
+    <sheet name="Indeces" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="173">
   <si>
     <t>level_row</t>
   </si>
@@ -50,12 +51,6 @@
     <t>col</t>
   </si>
   <si>
-    <t>commodity</t>
-  </si>
-  <si>
-    <t>activities</t>
-  </si>
-  <si>
     <t>Livestock (production)</t>
   </si>
   <si>
@@ -81,6 +76,486 @@
   </si>
   <si>
     <t>Maize (home consumed)</t>
+  </si>
+  <si>
+    <t>Commodities</t>
+  </si>
+  <si>
+    <t>Activities</t>
+  </si>
+  <si>
+    <t>Wheat (home consumed)</t>
+  </si>
+  <si>
+    <t>Rice (home consumed)</t>
+  </si>
+  <si>
+    <t>Other cereals (home consumed)</t>
+  </si>
+  <si>
+    <t>Roots &amp; tubers (home consumed)</t>
+  </si>
+  <si>
+    <t>Pulses &amp; oil seeds (home consumed)</t>
+  </si>
+  <si>
+    <t>Fruits (home consumed)</t>
+  </si>
+  <si>
+    <t>Vegetables (home consumed)</t>
+  </si>
+  <si>
+    <t>Beef (home consumed)</t>
+  </si>
+  <si>
+    <t>Dairy (home consumed)</t>
+  </si>
+  <si>
+    <t>Poultry (home consumed)</t>
+  </si>
+  <si>
+    <t>Sheep, goat and lamb for slaughter (home consumed)</t>
+  </si>
+  <si>
+    <t>Other livestock (home consumed)</t>
+  </si>
+  <si>
+    <t>Fishing (home consumed)</t>
+  </si>
+  <si>
+    <t>Sugar &amp; bakery &amp; confectionary (home consumed)</t>
+  </si>
+  <si>
+    <t>Beverages &amp; tobacco (home consumed)</t>
+  </si>
+  <si>
+    <t>Other manufactured food (home consumed)</t>
+  </si>
+  <si>
+    <t>Water (home consumed)</t>
+  </si>
+  <si>
+    <t>Wheat (marketed commodity)</t>
+  </si>
+  <si>
+    <t>Rice (marketed commodity)</t>
+  </si>
+  <si>
+    <t>Other cereals (marketed commodity)</t>
+  </si>
+  <si>
+    <t>Roots &amp; tubers (marketed commodity)</t>
+  </si>
+  <si>
+    <t>Pulses &amp; oil seeds (marketed commodity)</t>
+  </si>
+  <si>
+    <t>Fruits (marketed commodity)</t>
+  </si>
+  <si>
+    <t>Vegetables (marketed commodity)</t>
+  </si>
+  <si>
+    <t>Cotton (commodity)</t>
+  </si>
+  <si>
+    <t>Sugarcane (commodity)</t>
+  </si>
+  <si>
+    <t>Coffee (commodity)</t>
+  </si>
+  <si>
+    <t>Tea (commodity)</t>
+  </si>
+  <si>
+    <t>Tobacco (commodity)</t>
+  </si>
+  <si>
+    <t>Others crops (commodity)</t>
+  </si>
+  <si>
+    <t>Beef (marketed commodity)</t>
+  </si>
+  <si>
+    <t>Dairy (marketed commodity)</t>
+  </si>
+  <si>
+    <t>Poultry (marketed commodity)</t>
+  </si>
+  <si>
+    <t>Sheep, goat and lamb for slaughter (marketed commodity)</t>
+  </si>
+  <si>
+    <t>Other livestock (marketed commodity)</t>
+  </si>
+  <si>
+    <t>Fishing (marketed commodity)</t>
+  </si>
+  <si>
+    <t>Forestry (commodity)</t>
+  </si>
+  <si>
+    <t>Mining (commodity)</t>
+  </si>
+  <si>
+    <t>Meat &amp; dairy (commodity)</t>
+  </si>
+  <si>
+    <t>Grain milling (commodity)</t>
+  </si>
+  <si>
+    <t>Sugar &amp; bakery &amp; confectionary (marketed commodity)</t>
+  </si>
+  <si>
+    <t>Beverages &amp; tobacco (marketed commodity)</t>
+  </si>
+  <si>
+    <t>Other manufactured food (marketed commodity)</t>
+  </si>
+  <si>
+    <t>Textile &amp; clothing (commodity)</t>
+  </si>
+  <si>
+    <t>Leather &amp; footwear (commodity)</t>
+  </si>
+  <si>
+    <t>Wood &amp; paper (commodity)</t>
+  </si>
+  <si>
+    <t>Printing and publishing (commodity)</t>
+  </si>
+  <si>
+    <t>Petroleum (commodity)</t>
+  </si>
+  <si>
+    <t>Chemicals (commodity)</t>
+  </si>
+  <si>
+    <t>Fertilizers 0 Nitrogen (commodity)</t>
+  </si>
+  <si>
+    <t>Fertilizers 0 Phosphorus (commodity)</t>
+  </si>
+  <si>
+    <t>Fertilizers 0 Potassium (commodity)</t>
+  </si>
+  <si>
+    <t>Metals and machines (commodity)</t>
+  </si>
+  <si>
+    <t>Non metallic products (commodity)</t>
+  </si>
+  <si>
+    <t>Other manufacturers (commodity)</t>
+  </si>
+  <si>
+    <t>Water (marketed commodity)</t>
+  </si>
+  <si>
+    <t>Electricity (commodity)</t>
+  </si>
+  <si>
+    <t>Construction (commodity)</t>
+  </si>
+  <si>
+    <t>Trade (commodity)</t>
+  </si>
+  <si>
+    <t>Hotels (commodity)</t>
+  </si>
+  <si>
+    <t>Transport (commodity)</t>
+  </si>
+  <si>
+    <t>Communication (commodity)</t>
+  </si>
+  <si>
+    <t>Finance (commodity)</t>
+  </si>
+  <si>
+    <t>Real estate (commodity)</t>
+  </si>
+  <si>
+    <t>Other services (commodity)</t>
+  </si>
+  <si>
+    <t>Administration (commodity)</t>
+  </si>
+  <si>
+    <t>Health (commodity)</t>
+  </si>
+  <si>
+    <t>Education (commodity)</t>
+  </si>
+  <si>
+    <t>Extension services (commodity)</t>
+  </si>
+  <si>
+    <t>Nairobi</t>
+  </si>
+  <si>
+    <t>Mombasa</t>
+  </si>
+  <si>
+    <t>High Rainfall (household production)</t>
+  </si>
+  <si>
+    <t>Semi0Arid North (household production)</t>
+  </si>
+  <si>
+    <t>Semi0Arid South (household production)</t>
+  </si>
+  <si>
+    <t>Coast</t>
+  </si>
+  <si>
+    <t>Arid North</t>
+  </si>
+  <si>
+    <t>Arid South</t>
+  </si>
+  <si>
+    <t>High Rainfall (commercial production)</t>
+  </si>
+  <si>
+    <t>Semi0Arid North (commercial production)</t>
+  </si>
+  <si>
+    <t>Semi0Arid South (commercial production)</t>
+  </si>
+  <si>
+    <t>Food crops (production)</t>
+  </si>
+  <si>
+    <t>Cotton (production)</t>
+  </si>
+  <si>
+    <t>Sugarcane (production)</t>
+  </si>
+  <si>
+    <t>Coffee (production)</t>
+  </si>
+  <si>
+    <t>Tea (production)</t>
+  </si>
+  <si>
+    <t>Tobacco (production)</t>
+  </si>
+  <si>
+    <t>Others crops (production)</t>
+  </si>
+  <si>
+    <t>Dairy (production)</t>
+  </si>
+  <si>
+    <t>Fishing (production)</t>
+  </si>
+  <si>
+    <t>Forestry (production)</t>
+  </si>
+  <si>
+    <t>Mining (production)</t>
+  </si>
+  <si>
+    <t>Meat &amp; dairy (production)</t>
+  </si>
+  <si>
+    <t>Sugar &amp; bakery &amp; confectionary (production)</t>
+  </si>
+  <si>
+    <t>Beverages &amp; tobacco (production)</t>
+  </si>
+  <si>
+    <t>Other manufactured food (production)</t>
+  </si>
+  <si>
+    <t>Textile &amp; clothing (production)</t>
+  </si>
+  <si>
+    <t>Leather &amp; footwear (production)</t>
+  </si>
+  <si>
+    <t>Wood &amp; paper (production)</t>
+  </si>
+  <si>
+    <t>Printing and publishing (production)</t>
+  </si>
+  <si>
+    <t>Petroleum (production)</t>
+  </si>
+  <si>
+    <t>Chemicals (production)</t>
+  </si>
+  <si>
+    <t>Fertilizers 0 Nitrogen (production)</t>
+  </si>
+  <si>
+    <t>Fertilizers 0 Phosphorus (production)</t>
+  </si>
+  <si>
+    <t>Fertilizers 0 Potassium (production)</t>
+  </si>
+  <si>
+    <t>Metals and machines (production)</t>
+  </si>
+  <si>
+    <t>Non metallic products (production)</t>
+  </si>
+  <si>
+    <t>Other manufacturers (production)</t>
+  </si>
+  <si>
+    <t>Water (production)</t>
+  </si>
+  <si>
+    <t>Electricity (production)</t>
+  </si>
+  <si>
+    <t>Construction (production)</t>
+  </si>
+  <si>
+    <t>Trade (production)</t>
+  </si>
+  <si>
+    <t>Hotels (production)</t>
+  </si>
+  <si>
+    <t>Transport (production)</t>
+  </si>
+  <si>
+    <t>Communication (production)</t>
+  </si>
+  <si>
+    <t>Finance (production)</t>
+  </si>
+  <si>
+    <t>Real estate (production)</t>
+  </si>
+  <si>
+    <t>Other services (production)</t>
+  </si>
+  <si>
+    <t>Administration (production)</t>
+  </si>
+  <si>
+    <t>Health (production)</t>
+  </si>
+  <si>
+    <t>Education (production)</t>
+  </si>
+  <si>
+    <t>Extension services (production)</t>
+  </si>
+  <si>
+    <t>VA</t>
+  </si>
+  <si>
+    <t>Skilled labour 0 Nairobi</t>
+  </si>
+  <si>
+    <t>Semi0skilled labour 0 Nairobi</t>
+  </si>
+  <si>
+    <t>Unskilled labour 0 Nairobi</t>
+  </si>
+  <si>
+    <t>Skilled labour 0 Mombasa</t>
+  </si>
+  <si>
+    <t>Semi0skilled labour 0 Mombasa</t>
+  </si>
+  <si>
+    <t>Unskilled labour 0 Mombasa</t>
+  </si>
+  <si>
+    <t>Skilled labour 0 High Rainfall</t>
+  </si>
+  <si>
+    <t>Semi0skilled labour 0 High Rainfall</t>
+  </si>
+  <si>
+    <t>Skilled labour 0 Semi0Arid North</t>
+  </si>
+  <si>
+    <t>Semi0skilled labour 0 Semi0Arid North</t>
+  </si>
+  <si>
+    <t>Unskilled labour 0 Semi0Arid North</t>
+  </si>
+  <si>
+    <t>Skilled labour 0 Semi0Arid South</t>
+  </si>
+  <si>
+    <t>Semi0skilled labour 0 Semi0Arid South</t>
+  </si>
+  <si>
+    <t>Unskilled labour 0 Semi0Arid South</t>
+  </si>
+  <si>
+    <t>Skilled labour 0 Coast</t>
+  </si>
+  <si>
+    <t>Semi0skilled labour 0 Coast</t>
+  </si>
+  <si>
+    <t>Unskilled labour 0 Coast</t>
+  </si>
+  <si>
+    <t>Skilled labour 0 Arid North</t>
+  </si>
+  <si>
+    <t>Semi0skilled labour 0 Arid North</t>
+  </si>
+  <si>
+    <t>Unskilled labour 0 Arid North</t>
+  </si>
+  <si>
+    <t>Skilled labour 0 Arid South</t>
+  </si>
+  <si>
+    <t>Semi0skilled labour 0 Arid South</t>
+  </si>
+  <si>
+    <t>Unskilled labour 0 Arid South</t>
+  </si>
+  <si>
+    <t>Skilled labour 0 RoW</t>
+  </si>
+  <si>
+    <t>Semi0skilled labour 0 RoW</t>
+  </si>
+  <si>
+    <t>Unskilled labour 0 RoW</t>
+  </si>
+  <si>
+    <t>Land 0 irrigated (land factor)</t>
+  </si>
+  <si>
+    <t>Land 0 non0irrigated (land factor)</t>
+  </si>
+  <si>
+    <t>Livestock (factor)</t>
+  </si>
+  <si>
+    <t>Capital (agricultural)</t>
+  </si>
+  <si>
+    <t>Capital (non agricultural)</t>
+  </si>
+  <si>
+    <t>Direct taxes</t>
+  </si>
+  <si>
+    <t>Indirect taxes</t>
+  </si>
+  <si>
+    <t>Tariff on Africa</t>
+  </si>
+  <si>
+    <t>Tariff on ROW</t>
+  </si>
+  <si>
+    <t>Commodities,Activities</t>
   </si>
 </sst>
 </file>
@@ -130,7 +605,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -148,9 +623,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -469,7 +941,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,24 +961,22 @@
         <v>3</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="B2" s="7"/>
       <c r="C2" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E2" s="2">
         <v>10</v>
@@ -539,13 +1009,13 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -555,7 +1025,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -563,7 +1033,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>68</v>
       </c>
       <c r="C2" s="1">
         <v>100000000000000</v>
@@ -586,6 +1056,18 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4C950318-3C24-41EA-A9A6-38B5629C5A69}">
+          <x14:formula1>
+            <xm:f>Indeces!$A$2:$A$72</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -594,15 +1076,15 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
@@ -622,30 +1104,28 @@
         <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="B2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>9</v>
       </c>
       <c r="G2" s="5">
         <v>-0.5</v>
@@ -672,25 +1152,40 @@
       <c r="D6" s="2"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B6 D2:D6" xr:uid="{84BC44CA-847F-4EE5-8882-B1CE6219F7FC}">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B6 D3:D6" xr:uid="{84BC44CA-847F-4EE5-8882-B1CE6219F7FC}">
       <formula1>"commodity,activities"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{5E9F9CF7-75BB-4BAE-B1D3-9586E1D02A77}">
       <formula1>"Percentage, Absolute"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 D2" xr:uid="{C7302426-E37D-4FB6-888F-B69369A12DEE}">
+      <formula1>"Commodities,Activities"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6D80582A-72F6-4A68-A27C-AB8C3CBE9D27}">
+          <x14:formula1>
+            <xm:f>Indeces!$A$2:$A$126</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A46AE03-F2C9-4017-8F33-B063B461D8FD}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A6"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,7 +1198,7 @@
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
@@ -714,53 +1209,833 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>12</v>
+        <v>137</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="7" t="s">
         <v>13</v>
       </c>
+      <c r="D2" s="6"/>
       <c r="E2" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F2" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O9" s="1" t="s">
+        <v>172</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{6CEE8281-5D98-4CCF-93B5-298A9A185919}">
-      <formula1>"commodity,activities"</formula1>
+      <formula1>"Commodities,Activities"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{32F24E99-C857-4FF7-9B28-A412519FAC80}">
       <formula1>"Percentage, Absolute"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CEFB6047-CDFA-4073-8FC1-399DBE2DA67C}">
+          <x14:formula1>
+            <xm:f>Indeces!$C$2:$C$37</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{474C9CF5-5793-412F-8252-FEE72181A241}">
+          <x14:formula1>
+            <xm:f>Indeces!$A$2:$A$126</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A7BFC03-6CD2-49C0-AE9C-A9577AB4EC4A}">
+  <dimension ref="A1:C126"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F70" sqref="F70"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
excel file for pulping machin shock
</commit_message>
<xml_diff>
--- a/kenya_sut/Database/Shock.xlsx
+++ b/kenya_sut/Database/Shock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amin\Documents\GitHub\My Kenya\kenya_sut\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C142D8C-57E7-4A3D-BBF3-CE0C1D4BC3A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864FABFD-E8C0-4FCF-8FC6-46D49E08E9EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E3629C0E-F9DC-4B74-958E-3933B88A68DB}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="175">
   <si>
     <t>level_row</t>
   </si>
@@ -556,6 +556,12 @@
   </si>
   <si>
     <t>Commodities,Activities</t>
+  </si>
+  <si>
+    <t>cmdt</t>
+  </si>
+  <si>
+    <t>act</t>
   </si>
 </sst>
 </file>
@@ -1076,7 +1082,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1115,14 +1121,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="5" t="s">
-        <v>13</v>
-      </c>
       <c r="E2" s="6" t="s">
-        <v>4</v>
+        <v>86</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>7</v>
@@ -1172,7 +1180,7 @@
           <x14:formula1>
             <xm:f>Indeces!$A$2:$A$126</xm:f>
           </x14:formula1>
-          <xm:sqref>C2</xm:sqref>
+          <xm:sqref>C2 E2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1283,15 +1291,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A7BFC03-6CD2-49C0-AE9C-A9577AB4EC4A}">
-  <dimension ref="A1:C126"/>
+  <dimension ref="A1:E126"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F70" sqref="F70"/>
+    <sheetView topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="54" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -1301,122 +1314,173 @@
       <c r="C1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
+      <c r="B2" t="s">
+        <v>84</v>
+      </c>
       <c r="C2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
+      <c r="B3" t="s">
+        <v>85</v>
+      </c>
       <c r="C3" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
+      <c r="B4" t="s">
+        <v>86</v>
+      </c>
       <c r="C4" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
+      <c r="B5" t="s">
+        <v>87</v>
+      </c>
       <c r="C5" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
+      <c r="B6" t="s">
+        <v>88</v>
+      </c>
       <c r="C6" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
+      <c r="B7" t="s">
+        <v>89</v>
+      </c>
       <c r="C7" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
+      <c r="B8" t="s">
+        <v>90</v>
+      </c>
       <c r="C8" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>21</v>
       </c>
+      <c r="B9" t="s">
+        <v>91</v>
+      </c>
       <c r="C9" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
+      <c r="B10" t="s">
+        <v>92</v>
+      </c>
       <c r="C10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
+      <c r="B11" t="s">
+        <v>93</v>
+      </c>
       <c r="C11" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
+      <c r="B12" t="s">
+        <v>94</v>
+      </c>
       <c r="C12" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
+      <c r="B13" t="s">
+        <v>95</v>
+      </c>
       <c r="C13" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
+      <c r="B14" t="s">
+        <v>96</v>
+      </c>
       <c r="C14" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
+      <c r="B15" t="s">
+        <v>97</v>
+      </c>
       <c r="C15" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>98</v>
       </c>
       <c r="C16" t="s">
         <v>150</v>
@@ -1426,6 +1490,9 @@
       <c r="A17" t="s">
         <v>29</v>
       </c>
+      <c r="B17" t="s">
+        <v>99</v>
+      </c>
       <c r="C17" t="s">
         <v>151</v>
       </c>
@@ -1434,6 +1501,9 @@
       <c r="A18" t="s">
         <v>30</v>
       </c>
+      <c r="B18" t="s">
+        <v>100</v>
+      </c>
       <c r="C18" t="s">
         <v>152</v>
       </c>
@@ -1442,6 +1512,9 @@
       <c r="A19" t="s">
         <v>31</v>
       </c>
+      <c r="B19" t="s">
+        <v>101</v>
+      </c>
       <c r="C19" t="s">
         <v>153</v>
       </c>
@@ -1450,6 +1523,9 @@
       <c r="A20" t="s">
         <v>5</v>
       </c>
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
       <c r="C20" t="s">
         <v>154</v>
       </c>
@@ -1458,6 +1534,9 @@
       <c r="A21" t="s">
         <v>32</v>
       </c>
+      <c r="B21" t="s">
+        <v>102</v>
+      </c>
       <c r="C21" t="s">
         <v>155</v>
       </c>
@@ -1466,6 +1545,9 @@
       <c r="A22" t="s">
         <v>33</v>
       </c>
+      <c r="B22" t="s">
+        <v>103</v>
+      </c>
       <c r="C22" t="s">
         <v>156</v>
       </c>
@@ -1474,6 +1556,9 @@
       <c r="A23" t="s">
         <v>34</v>
       </c>
+      <c r="B23" t="s">
+        <v>104</v>
+      </c>
       <c r="C23" t="s">
         <v>157</v>
       </c>
@@ -1482,6 +1567,9 @@
       <c r="A24" t="s">
         <v>35</v>
       </c>
+      <c r="B24" t="s">
+        <v>105</v>
+      </c>
       <c r="C24" t="s">
         <v>158</v>
       </c>
@@ -1490,6 +1578,9 @@
       <c r="A25" t="s">
         <v>36</v>
       </c>
+      <c r="B25" t="s">
+        <v>106</v>
+      </c>
       <c r="C25" t="s">
         <v>159</v>
       </c>
@@ -1498,6 +1589,9 @@
       <c r="A26" t="s">
         <v>37</v>
       </c>
+      <c r="B26" t="s">
+        <v>11</v>
+      </c>
       <c r="C26" t="s">
         <v>160</v>
       </c>
@@ -1506,6 +1600,9 @@
       <c r="A27" t="s">
         <v>38</v>
       </c>
+      <c r="B27" t="s">
+        <v>107</v>
+      </c>
       <c r="C27" t="s">
         <v>161</v>
       </c>
@@ -1514,6 +1611,9 @@
       <c r="A28" t="s">
         <v>39</v>
       </c>
+      <c r="B28" t="s">
+        <v>108</v>
+      </c>
       <c r="C28" t="s">
         <v>162</v>
       </c>
@@ -1522,6 +1622,9 @@
       <c r="A29" t="s">
         <v>40</v>
       </c>
+      <c r="B29" t="s">
+        <v>109</v>
+      </c>
       <c r="C29" t="s">
         <v>163</v>
       </c>
@@ -1530,6 +1633,9 @@
       <c r="A30" t="s">
         <v>41</v>
       </c>
+      <c r="B30" t="s">
+        <v>110</v>
+      </c>
       <c r="C30" t="s">
         <v>164</v>
       </c>
@@ -1538,6 +1644,9 @@
       <c r="A31" t="s">
         <v>42</v>
       </c>
+      <c r="B31" t="s">
+        <v>111</v>
+      </c>
       <c r="C31" t="s">
         <v>165</v>
       </c>
@@ -1546,6 +1655,9 @@
       <c r="A32" t="s">
         <v>43</v>
       </c>
+      <c r="B32" t="s">
+        <v>112</v>
+      </c>
       <c r="C32" t="s">
         <v>166</v>
       </c>
@@ -1554,6 +1666,9 @@
       <c r="A33" t="s">
         <v>44</v>
       </c>
+      <c r="B33" t="s">
+        <v>113</v>
+      </c>
       <c r="C33" t="s">
         <v>167</v>
       </c>
@@ -1562,6 +1677,9 @@
       <c r="A34" t="s">
         <v>45</v>
       </c>
+      <c r="B34" t="s">
+        <v>114</v>
+      </c>
       <c r="C34" t="s">
         <v>168</v>
       </c>
@@ -1570,6 +1688,9 @@
       <c r="A35" t="s">
         <v>46</v>
       </c>
+      <c r="B35" t="s">
+        <v>115</v>
+      </c>
       <c r="C35" t="s">
         <v>169</v>
       </c>
@@ -1578,6 +1699,9 @@
       <c r="A36" t="s">
         <v>47</v>
       </c>
+      <c r="B36" t="s">
+        <v>116</v>
+      </c>
       <c r="C36" t="s">
         <v>170</v>
       </c>
@@ -1586,6 +1710,9 @@
       <c r="A37" t="s">
         <v>48</v>
       </c>
+      <c r="B37" t="s">
+        <v>117</v>
+      </c>
       <c r="C37" t="s">
         <v>171</v>
       </c>
@@ -1594,133 +1721,187 @@
       <c r="A38" t="s">
         <v>49</v>
       </c>
+      <c r="B38" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>50</v>
       </c>
+      <c r="B39" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>51</v>
       </c>
+      <c r="B40" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>52</v>
       </c>
+      <c r="B41" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>53</v>
       </c>
+      <c r="B42" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>54</v>
       </c>
+      <c r="B43" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>55</v>
       </c>
+      <c r="B44" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>56</v>
       </c>
+      <c r="B45" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>57</v>
       </c>
+      <c r="B46" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>58</v>
       </c>
+      <c r="B47" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>75</v>
       </c>
@@ -2036,6 +2217,14 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{3F3464B1-0512-4134-BDA3-AE4ABA7C86A2}">
+      <formula1>$A$2:$A$72</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{CA259FB8-62DD-434E-A141-D6F6A3C773B4}">
+      <formula1>$B$2:$B$55</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>